<commit_message>
select uptade e insert
</commit_message>
<xml_diff>
--- a/Mapa.xlsx
+++ b/Mapa.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Borking\Desktop\cualquiera\BaseDatosAplicada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E96D6D63-F8C0-4244-B939-03992A3D12C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027212B7-8D3C-4AC6-8934-18BB7B3523D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{B89BA862-B6DF-4216-A4AF-79BF6F40919E}"/>
+    <workbookView xWindow="27690" yWindow="2100" windowWidth="14670" windowHeight="8325" xr2:uid="{B89BA862-B6DF-4216-A4AF-79BF6F40919E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
-  <si>
-    <t>Fruteria Lulu</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>NIT</t>
   </si>
@@ -37,9 +33,6 @@
     <t>Dirección</t>
   </si>
   <si>
-    <t>Numero C</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -79,9 +72,6 @@
     <t>Direccion</t>
   </si>
   <si>
-    <t>Domiciliarios</t>
-  </si>
-  <si>
     <t>C.C</t>
   </si>
   <si>
@@ -107,13 +97,49 @@
   </si>
   <si>
     <t>Valor total</t>
+  </si>
+  <si>
+    <t>Id_Cliente</t>
+  </si>
+  <si>
+    <t>FK</t>
+  </si>
+  <si>
+    <t>Id_proveedor</t>
+  </si>
+  <si>
+    <t>Id_Pdv</t>
+  </si>
+  <si>
+    <t>Id_Inventario</t>
+  </si>
+  <si>
+    <t>Empleado</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Id_Empleado</t>
+  </si>
+  <si>
+    <t>Fruteria Lulu Database</t>
+  </si>
+  <si>
+    <t>Telefono_Empresa</t>
+  </si>
+  <si>
+    <t>Razon_Social</t>
+  </si>
+  <si>
+    <t>Apellido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,16 +147,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,8 +161,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -176,11 +200,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,19 +270,50 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -525,270 +630,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD14DB6-5E36-4443-9AFA-6AE01786887E}">
-  <dimension ref="C4:R30"/>
+  <dimension ref="E3:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="8"/>
+    <row r="3" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="I3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="14"/>
       <c r="G4" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="8"/>
+        <v>11</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="14"/>
       <c r="K4" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="P4" s="8"/>
       <c r="Q4" s="9"/>
       <c r="R4" s="10"/>
     </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="5" t="s">
+    <row r="5" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="J5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="7" t="s">
+      <c r="N5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="2"/>
+      <c r="J7" s="7"/>
       <c r="K7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="2" t="s">
-        <v>25</v>
+      <c r="M7" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+    <row r="8" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="G8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="21"/>
       <c r="I8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="J8" s="7"/>
       <c r="K8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="17"/>
+    </row>
+    <row r="9" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="J9" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="K9" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="M9" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+      <c r="G10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="23"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="M10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="3"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+    <row r="11" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="M11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="3"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="G12" s="1"/>
+    <row r="12" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="G12" s="23"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="M12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="3"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:18" x14ac:dyDescent="0.25">
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="M13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:18" x14ac:dyDescent="0.25">
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="M14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:18" x14ac:dyDescent="0.25">
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="M15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:18" x14ac:dyDescent="0.25">
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="M16" s="12"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
@@ -870,7 +1000,6 @@
       <c r="O23" s="1"/>
     </row>
     <row r="24" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -881,7 +1010,6 @@
       <c r="O24" s="1"/>
     </row>
     <row r="25" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -892,7 +1020,6 @@
       <c r="O25" s="1"/>
     </row>
     <row r="26" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -903,7 +1030,6 @@
       <c r="O26" s="1"/>
     </row>
     <row r="27" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -914,7 +1040,6 @@
       <c r="O27" s="1"/>
     </row>
     <row r="28" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -925,7 +1050,6 @@
       <c r="O28" s="1"/>
     </row>
     <row r="29" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -943,19 +1067,28 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
       <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G31" s="1"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M33" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>